<commit_message>
chore: update forms to use new template
</commit_message>
<xml_diff>
--- a/CHT_FORM_TEMPLATE.xlsx
+++ b/CHT_FORM_TEMPLATE.xlsx
@@ -832,11 +832,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1116,10 +1116,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I29" activeCellId="0" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.63"/>
@@ -1221,17 +1221,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="0"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="5"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="0"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:X13 A28:X10000 A27:B27 D27:X27 A17:X26 A14:D16 F14:X16">
@@ -1330,7 +1327,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.63"/>
@@ -1415,12 +1412,12 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,20 +1438,20 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="8" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20241028152830</v>
-      </c>
-      <c r="D2" s="6" t="s">
+        <v>20250213143911</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: update forms to use new template (#17)
</commit_message>
<xml_diff>
--- a/CHT_FORM_TEMPLATE.xlsx
+++ b/CHT_FORM_TEMPLATE.xlsx
@@ -832,11 +832,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1116,10 +1116,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I29" activeCellId="0" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.63"/>
@@ -1221,17 +1221,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="0"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="5"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="0"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:X13 A28:X10000 A27:B27 D27:X27 A17:X26 A14:D16 F14:X16">
@@ -1330,7 +1327,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.63"/>
@@ -1415,12 +1412,12 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,20 +1438,20 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="8" t="str">
         <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20241028152830</v>
-      </c>
-      <c r="D2" s="6" t="s">
+        <v>20250213143911</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>